<commit_message>
Updated Month output from export and year output from export. Also added transation tab with all transaction data and their category.  Resolved bug with up to month option averaging functionality.
</commit_message>
<xml_diff>
--- a/Expenses.xlsx
+++ b/Expenses.xlsx
@@ -8,6 +8,19 @@
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="January" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="February" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="March" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="April" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="May" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="June" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="July" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="August" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="September" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="October" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="November" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="December" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="Transactions" sheetId="14" state="visible" r:id="rId14"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,7 +30,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -38,6 +51,11 @@
     <font>
       <color rgb="0003fc6f"/>
       <sz val="12"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="0003fc6f"/>
+      <sz val="24"/>
     </font>
   </fonts>
   <fills count="2">
@@ -60,7 +78,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
@@ -70,6 +88,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -436,7 +457,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,7 +473,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Current Monthly Spent</t>
+          <t>Current Average Monthly Spendings</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -460,16 +481,26 @@
           <t>Allocated Monthly Spendings</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Current Yearly Spendings</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Allocated Yearly Spendings</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Food</t>
+          <t>test</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
-          <t>16.54</t>
+          <t>30.0</t>
         </is>
       </c>
       <c r="C2" s="3" t="inlineStr">
@@ -477,25 +508,697 @@
           <t>0</t>
         </is>
       </c>
+      <c r="D2" s="3" t="inlineStr">
+        <is>
+          <t>30.0</t>
+        </is>
+      </c>
+      <c r="E2" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>Month of September Expenses</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="C2" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>Month of October Expenses</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="C2" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>Month of November Expenses</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="C2" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>Month of December Expenses</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="C2" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>* Cash App Cash App        PPD</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>07/10/24</t>
+        </is>
+      </c>
+      <c r="D1" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Interest Deposit</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>07/31/24</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>0.04</t>
+        </is>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t>rent</t>
-        </is>
-      </c>
-      <c r="B3" s="3" t="inlineStr">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Service Charge</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>07/31/24</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Interest Deposit</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>09/02/24</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>0.05</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Interest Deposit</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>09/30/24</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
         <is>
           <t>0.03</t>
         </is>
       </c>
-      <c r="C3" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Interest Deposit</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>10/31/24</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>0.03</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>Month of January Expenses</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="C2" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>Month of February Expenses</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="C2" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>Month of March Expenses</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="C2" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>Month of April Expenses</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="C2" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>Month of May Expenses</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="C2" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>Month of June Expenses</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="C2" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>Month of July Expenses</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>30.0</t>
+        </is>
+      </c>
+      <c r="C2" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>Month of August Expenses</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="C2" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>